<commit_message>
Atualização 05/10 - Troca da Base de Dados
</commit_message>
<xml_diff>
--- a/data/LCDataDictionary.xlsx
+++ b/data/LCDataDictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leova\Desktop\Repositório Atualizado\Repositorio_Data_Science\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leova\Desktop\Projetos\05_modelo_risco_de_credito\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DF97EC-160A-4B8B-B641-16A987BE63F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD02CDD-199F-448D-87C7-707895571382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,17 +19,11 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$B$89</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$B$1:$B$81</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -38,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="375">
   <si>
     <t>id</t>
   </si>
@@ -927,13 +921,250 @@
   </si>
   <si>
     <t>total_cu_tl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrição </t>
+  </si>
+  <si>
+    <t>O estado fornecido pelo mutuário no pedido de empréstimo</t>
+  </si>
+  <si>
+    <t>A renda anual declarada pelo próprio mutuário durante o registro.</t>
+  </si>
+  <si>
+    <t>A renda anual combinada autodeclarada fornecida pelos co-mutuários durante o registro</t>
+  </si>
+  <si>
+    <t>Indica se o empréstimo é um pedido individual ou um pedido conjunto com dois co-mutuários</t>
+  </si>
+  <si>
+    <t>pós cobrança da taxa de cobrança</t>
+  </si>
+  <si>
+    <t>Número de coletas em 12 meses excluindo coletas médicas</t>
+  </si>
+  <si>
+    <t>O número de incidências de inadimplência vencidas há mais de 30 dias no arquivo de crédito do mutuário nos últimos 2 anos</t>
+  </si>
+  <si>
+    <t>Descrição do empréstimo fornecida pelo mutuário</t>
+  </si>
+  <si>
+    <t>Uma razão calculada utilizando o total dos pagamentos mensais da dívida do mutuário sobre o total das obrigações da dívida, excluindo a hipoteca e o empréstimo em ML solicitado, dividido pelo rendimento mensal autodeclarado pelo mutuário.</t>
+  </si>
+  <si>
+    <t>Um índice calculado usando o total de pagamentos mensais dos co-mutuários sobre o total das obrigações da dívida, excluindo hipotecas e o empréstimo em ML solicitado, dividido pela renda mensal combinada declarada pelos co-mutuários</t>
+  </si>
+  <si>
+    <t>O mês em que a primeira linha de crédito informada pelo mutuário foi aberta</t>
+  </si>
+  <si>
+    <t>Duração do emprego em anos. Os valores possíveis estão entre 0 e 10, onde 0 significa menos de um ano e 10 significa dez ou mais anos.</t>
+  </si>
+  <si>
+    <t>O cargo fornecido pelo Mutuário ao solicitar o empréstimo.*</t>
+  </si>
+  <si>
+    <t>A faixa limite superior à qual pertence o FICO do mutuário na originação do empréstimo.</t>
+  </si>
+  <si>
+    <t>O limite inferior ao qual pertence o FICO do mutuário na originação do empréstimo.</t>
+  </si>
+  <si>
+    <t>O valor total comprometido com esse empréstimo naquele momento.</t>
+  </si>
+  <si>
+    <t>O montante total comprometido pelos investidores para esse empréstimo naquele momento.</t>
+  </si>
+  <si>
+    <t>Grau de empréstimo atribuído a LC</t>
+  </si>
+  <si>
+    <t>O status de propriedade residencial fornecido pelo mutuário durante o registro. Nossos valores são: ALUGUEL, PRÓPRIO, HIPOTECA, OUTROS.</t>
+  </si>
+  <si>
+    <t>Um ID exclusivo atribuído ao LC para a listagem de empréstimos.</t>
+  </si>
+  <si>
+    <t>O status de listagem inicial do empréstimo. Os valores possíveis são – W, ​​F</t>
+  </si>
+  <si>
+    <t>O número de consultas nos últimos 6 meses (excluindo consultas sobre automóveis e hipotecas)</t>
+  </si>
+  <si>
+    <t>O pagamento mensal devido pelo mutuário se o empréstimo for originado.</t>
+  </si>
+  <si>
+    <t>Taxa de juros do empréstimo</t>
+  </si>
+  <si>
+    <t>Indica se a renda foi apurada por LC, não apurada, ou se a fonte de renda foi apurada</t>
+  </si>
+  <si>
+    <t>O mês em que o empréstimo foi financiado</t>
+  </si>
+  <si>
+    <t>No mês mais recente, LC retirou crédito para este empréstimo</t>
+  </si>
+  <si>
+    <t>A faixa limite superior à qual pertence o último FICO retirado do mutuário.</t>
+  </si>
+  <si>
+    <t>O limite inferior ao qual pertence o último FICO retirado do mutuário.</t>
+  </si>
+  <si>
+    <t>Último valor total do pagamento recebido</t>
+  </si>
+  <si>
+    <t>O pagamento do mês passado foi recebido</t>
+  </si>
+  <si>
+    <t>O valor listado do empréstimo solicitado pelo mutuário. Se em algum momento o departamento de crédito reduzir o valor do empréstimo, isso será refletido nesse valor.</t>
+  </si>
+  <si>
+    <t>Situação atual do empréstimo</t>
+  </si>
+  <si>
+    <t>Um ID exclusivo atribuído ao LC para o membro mutuário.</t>
+  </si>
+  <si>
+    <t>O número de meses desde a última inadimplência do mutuário.</t>
+  </si>
+  <si>
+    <t>Meses desde a classificação mais recente de 90 dias ou pior</t>
+  </si>
+  <si>
+    <t>O número de meses desde o último registro público.</t>
+  </si>
+  <si>
+    <t>Próxima data de pagamento agendada</t>
+  </si>
+  <si>
+    <t>O número de linhas de crédito abertas no arquivo de crédito do mutuário.</t>
+  </si>
+  <si>
+    <t>Capital restante pendente para o valor total financiado</t>
+  </si>
+  <si>
+    <t>Capital restante em aberto para parte do valor total financiado pelos investidores</t>
+  </si>
+  <si>
+    <t>"policy_code disponível publicamente=1 ; novos produtos não disponíveis publicamente policy_code=2"</t>
+  </si>
+  <si>
+    <t>Número de registros públicos depreciativos</t>
+  </si>
+  <si>
+    <t>Uma categoria fornecida pelo mutuário para a solicitação de empréstimo.</t>
+  </si>
+  <si>
+    <t>Indica se um plano de pagamento foi implementado para o empréstimo</t>
+  </si>
+  <si>
+    <t>pós cobrança da recuperação bruta</t>
+  </si>
+  <si>
+    <t>Saldo rotativo de crédito total</t>
+  </si>
+  <si>
+    <t>Taxa de utilização da linha rotativa ou a quantidade de crédito que o mutuário está usando em relação a todo o crédito rotativo disponível.</t>
+  </si>
+  <si>
+    <t>Subclasse de empréstimo atribuído a LC</t>
+  </si>
+  <si>
+    <t>O número de pagamentos do empréstimo. Os valores estão em meses e podem ser 36 ou 60.</t>
+  </si>
+  <si>
+    <t>O título do empréstimo fornecido pelo mutuário</t>
+  </si>
+  <si>
+    <t>O número total de linhas de crédito atualmente no arquivo de crédito do mutuário</t>
+  </si>
+  <si>
+    <t>Pagamentos recebidos até o momento pelo valor total financiado</t>
+  </si>
+  <si>
+    <t>Pagamentos recebidos até o momento referentes a parte do valor total financiado pelos investidores</t>
+  </si>
+  <si>
+    <t>Juros recebidos até o momento</t>
+  </si>
+  <si>
+    <t>Taxas atrasadas recebidas até o momento</t>
+  </si>
+  <si>
+    <t>Principal recebido até o momento</t>
+  </si>
+  <si>
+    <t>URL da página LC com dados de listagem.</t>
+  </si>
+  <si>
+    <t>Indica se a renda conjunta dos co-mutuários foi verificada pelo LC, não verificada, ou se a fonte de renda foi verificada</t>
+  </si>
+  <si>
+    <t>Os primeiros 3 números do CEP fornecido pelo mutuário no pedido de empréstimo.</t>
+  </si>
+  <si>
+    <t>Número de negociações abertas nos últimos 6 meses</t>
+  </si>
+  <si>
+    <t>Número de negociações parceladas atualmente ativas</t>
+  </si>
+  <si>
+    <t>Número de contas parceladas abertas nos últimos 12 meses</t>
+  </si>
+  <si>
+    <t>Número de contas parceladas abertas nos últimos 24 meses</t>
+  </si>
+  <si>
+    <t>Meses desde a abertura das contas parceladas mais recentes</t>
+  </si>
+  <si>
+    <t>Saldo atual total de todas as contas parceladas</t>
+  </si>
+  <si>
+    <t>Proporção entre o saldo atual total e o limite de crédito/crédito alto em todas as contas de instalação</t>
+  </si>
+  <si>
+    <t>Número de negociações rotativas abertas nos últimos 12 meses</t>
+  </si>
+  <si>
+    <t>Número de negociações rotativas abertas nos últimos 24 meses</t>
+  </si>
+  <si>
+    <t>Saldo atual máximo devido em todas as contas rotativas</t>
+  </si>
+  <si>
+    <t>Saldo até o limite de crédito em todas as negociações</t>
+  </si>
+  <si>
+    <t>Total de crédito/limite de crédito alto rotativo</t>
+  </si>
+  <si>
+    <t>Número de consultas sobre finanças pessoais</t>
+  </si>
+  <si>
+    <t>Número de negociações financeiras</t>
+  </si>
+  <si>
+    <t>Número de consultas de crédito nos últimos 12 meses</t>
+  </si>
+  <si>
+    <t>O número de contas nas quais o mutuário está atualmente inadimplente.</t>
+  </si>
+  <si>
+    <t>Valores totais de cobrança já devidos</t>
+  </si>
+  <si>
+    <t>Saldo atual total de todas as contas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1116,6 +1347,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1310,7 +1549,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1453,15 +1692,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1567,17 +1797,17 @@
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="88">
@@ -1681,6 +1911,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="dimg_3" descr="Ícone &quot;Verificada pela comunidade&quot;">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{683D6FD1-7D2D-8BC6-CC0F-60803156F86E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9925050" y="22945725"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1975,671 +2271,901 @@
   </sheetPr>
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118.140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="118.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118.140625" style="11" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="118.140625" style="11" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>49</v>
       </c>
+      <c r="C1" s="12" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>242</v>
       </c>
+      <c r="C2" s="11" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>260</v>
       </c>
+      <c r="C3" s="11" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>255</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>266</v>
       </c>
+      <c r="C4" s="11" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>253</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>254</v>
       </c>
+      <c r="C5" s="11" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>227</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>225</v>
       </c>
+      <c r="C6" s="11" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>107</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>132</v>
       </c>
+      <c r="C7" s="11" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>55</v>
       </c>
+      <c r="C8" s="11" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>57</v>
       </c>
+      <c r="C9" s="11" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="C10" s="11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>256</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>257</v>
       </c>
+      <c r="C11" s="11" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>250</v>
       </c>
+      <c r="C12" s="11" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>59</v>
       </c>
+      <c r="C13" s="11" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>167</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>168</v>
       </c>
+      <c r="C14" s="11" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="11" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="11" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="C17" s="11" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>222</v>
       </c>
+      <c r="C18" s="11" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>61</v>
       </c>
+      <c r="C19" s="11" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>62</v>
       </c>
+      <c r="C20" s="11" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>63</v>
       </c>
+      <c r="C21" s="11" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>64</v>
       </c>
+      <c r="C22" s="11" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>263</v>
       </c>
+      <c r="C23" s="11" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>65</v>
       </c>
+      <c r="C24" s="11" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>88</v>
       </c>
+      <c r="C25" s="11" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>223</v>
       </c>
+      <c r="C26" s="11" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>249</v>
       </c>
+      <c r="C27" s="11" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>252</v>
       </c>
+      <c r="C28" s="11" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="C29" s="9"/>
+      <c r="C29" s="11" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="C30" s="9"/>
+      <c r="C30" s="11" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>98</v>
       </c>
+      <c r="C31" s="11" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="C32" s="11" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="C33" s="11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="C34" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="C35" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="C36" s="11" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>109</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="C37" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="C38" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="C39" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="C40" s="11" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="C41" s="11" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="C42" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
         <v>130</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="C43" s="11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="C44" s="11" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="C45" s="11" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="C46" s="11" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>226</v>
       </c>
       <c r="B47" s="11" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+      <c r="C47" s="11" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="C48" s="11" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="11" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="C49" s="11" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="C50" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+      <c r="C51" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B52" s="11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
+      <c r="C52" s="11" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>34</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
+      <c r="C53" s="11" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
+      <c r="C54" s="11" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>39</v>
       </c>
       <c r="B55" s="11" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
+      <c r="C55" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+      <c r="C56" s="11" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+      <c r="C57" s="11" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="C58" s="11" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B59" s="11" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="C59" s="11" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
         <v>258</v>
       </c>
       <c r="B60" s="11" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="C60" s="11" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
         <v>248</v>
       </c>
       <c r="B61" s="11" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
+      <c r="C61" s="11" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
         <v>267</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
+      <c r="C62" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>269</v>
       </c>
       <c r="B63" s="11" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
+      <c r="C63" s="11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
         <v>271</v>
       </c>
       <c r="B64" s="11" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+      <c r="C64" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
         <v>273</v>
       </c>
       <c r="B65" s="11" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
+      <c r="C65" s="11" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
         <v>275</v>
       </c>
       <c r="B66" s="11" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
+      <c r="C66" s="11" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
         <v>277</v>
       </c>
       <c r="B67" s="11" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+      <c r="C67" s="11" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="s">
         <v>279</v>
       </c>
       <c r="B68" s="11" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
+      <c r="C68" s="11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
         <v>281</v>
       </c>
       <c r="B69" s="11" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
+      <c r="C69" s="11" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
         <v>283</v>
       </c>
       <c r="B70" s="11" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
+      <c r="C70" s="11" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
         <v>285</v>
       </c>
       <c r="B71" s="11" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
+      <c r="C71" s="11" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
         <v>287</v>
       </c>
       <c r="B72" s="11" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
+      <c r="C72" s="11" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
         <v>218</v>
       </c>
       <c r="B73" s="11" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
+      <c r="C73" s="11" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
         <v>289</v>
       </c>
       <c r="B74" s="11" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
+      <c r="C74" s="11" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
         <v>295</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
+      <c r="C75" s="11" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
         <v>291</v>
       </c>
       <c r="B76" s="11" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
+      <c r="C76" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
         <v>293</v>
       </c>
       <c r="B77" s="11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
+      <c r="C77" s="11" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
         <v>129</v>
       </c>
       <c r="B78" s="11" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
+      <c r="C78" s="11" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
         <v>114</v>
       </c>
       <c r="B79" s="11" t="s">
         <v>156</v>
       </c>
+      <c r="C79" s="11" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="12" t="s">
+      <c r="B81" s="11" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B57" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B61">
-      <sortCondition ref="A1:A61"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="B1:B81" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="64" orientation="portrait" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Atualização 07/10 - Segmentação das Variáveis e Início das Análises
</commit_message>
<xml_diff>
--- a/data/LCDataDictionary.xlsx
+++ b/data/LCDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leova\Desktop\Projetos\05_modelo_risco_de_credito\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD02CDD-199F-448D-87C7-707895571382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7B79D8-995C-473A-B647-668AECA21A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="38640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$B$89</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$B$1:$B$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$C$81</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="376">
   <si>
     <t>id</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>emp_length</t>
-  </si>
-  <si>
-    <t>home_ownership</t>
   </si>
   <si>
     <t>annual_inc</t>
@@ -992,9 +989,6 @@
     <t>O número de consultas nos últimos 6 meses (excluindo consultas sobre automóveis e hipotecas)</t>
   </si>
   <si>
-    <t>O pagamento mensal devido pelo mutuário se o empréstimo for originado.</t>
-  </si>
-  <si>
     <t>Taxa de juros do empréstimo</t>
   </si>
   <si>
@@ -1016,9 +1010,6 @@
     <t>Último valor total do pagamento recebido</t>
   </si>
   <si>
-    <t>O pagamento do mês passado foi recebido</t>
-  </si>
-  <si>
     <t>O valor listado do empréstimo solicitado pelo mutuário. Se em algum momento o departamento de crédito reduzir o valor do empréstimo, isso será refletido nesse valor.</t>
   </si>
   <si>
@@ -1158,6 +1149,18 @@
   </si>
   <si>
     <t>Saldo atual total de todas as contas</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>continua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data do último pagamento </t>
+  </si>
+  <si>
+    <t>O pagamento mensal devido pelo mutuário se o empréstimo for originado. (Em termos simples, a originação de um empréstimo é o ponto de partida, onde o mutuário (a pessoa ou entidade que pede o empréstimo) solicita o empréstimo a um credor (a instituição financeira ou pessoa que empresta o dinheiro) e o credor avalia a solicitação, verifica a elegibilidade do mutuário e decide se concederá ou não o empréstimo.)</t>
   </si>
 </sst>
 </file>
@@ -2269,195 +2272,207 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118.140625" style="11" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="66.7109375" style="11" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="118.140625" style="11" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="D2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="D3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="D5" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B10" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="B11" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="B12" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="C14" s="11" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="11" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C16" s="11" t="s">
         <v>310</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2465,10 +2480,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2476,10 +2491,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2487,21 +2502,18 @@
         <v>8</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2509,43 +2521,43 @@
         <v>0</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>319</v>
+        <v>375</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2553,87 +2565,87 @@
         <v>6</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>327</v>
+        <v>374</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -2641,21 +2653,21 @@
         <v>2</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2663,164 +2675,164 @@
         <v>1</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2828,10 +2840,10 @@
         <v>9</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2839,333 +2851,333 @@
         <v>5</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B60" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="B60" s="11" t="s">
-        <v>259</v>
-      </c>
       <c r="C60" s="11" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="B62" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>268</v>
-      </c>
       <c r="C62" s="11" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B63" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="B63" s="11" t="s">
-        <v>270</v>
-      </c>
       <c r="C63" s="11" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="B64" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="B64" s="11" t="s">
-        <v>272</v>
-      </c>
       <c r="C64" s="11" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B65" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="B65" s="11" t="s">
-        <v>274</v>
-      </c>
       <c r="C65" s="11" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B66" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="B66" s="11" t="s">
-        <v>276</v>
-      </c>
       <c r="C66" s="11" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="B67" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="B67" s="11" t="s">
-        <v>278</v>
-      </c>
       <c r="C67" s="11" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="B68" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="B68" s="11" t="s">
-        <v>280</v>
-      </c>
       <c r="C68" s="11" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B69" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="B69" s="11" t="s">
-        <v>282</v>
-      </c>
       <c r="C69" s="11" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B70" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="B70" s="11" t="s">
-        <v>284</v>
-      </c>
       <c r="C70" s="11" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B71" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="B71" s="11" t="s">
-        <v>286</v>
-      </c>
       <c r="C71" s="11" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="B72" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="B72" s="11" t="s">
-        <v>288</v>
-      </c>
       <c r="C72" s="11" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="B74" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="B74" s="11" t="s">
-        <v>290</v>
-      </c>
       <c r="C74" s="11" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B76" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="B76" s="11" t="s">
-        <v>292</v>
-      </c>
       <c r="C76" s="11" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B81" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C81" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">
     <sortCondition ref="A2:A101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="64" orientation="portrait" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="64" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3192,226 +3204,226 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" t="s">
         <v>256</v>
-      </c>
-      <c r="B19" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -3419,15 +3431,15 @@
         <v>8</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -3435,31 +3447,31 @@
         <v>0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B34" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3467,367 +3479,367 @@
         <v>7</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -3835,220 +3847,220 @@
         <v>5</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>277</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B109" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -4086,82 +4098,82 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" t="s">
         <v>244</v>
-      </c>
-      <c r="B5" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finalização Análise de Variáveis dos Clientes  29/10
</commit_message>
<xml_diff>
--- a/data/LCDataDictionary.xlsx
+++ b/data/LCDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leova\Desktop\Projetos\05_modelo_risco_de_credito\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7B79D8-995C-473A-B647-668AECA21A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5A2D05-7B74-41F0-87A6-A192179CC30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="38640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="16200" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -2276,7 +2276,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2312,7 +2312,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>254</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>252</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>23</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>166</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>25</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>3</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>61</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>34</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>26</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>12</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>46</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>47</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>2</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>27</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>29</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>18</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>15</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>5</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>33</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>38</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>247</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>270</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>272</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>278</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>292</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B81" s="11" t="s">
         <v>168</v>
       </c>

</xml_diff>

<commit_message>
Inicio do Processo de Modelagem - Feature Engineering Completo 16/11 - Madrugada
</commit_message>
<xml_diff>
--- a/data/LCDataDictionary.xlsx
+++ b/data/LCDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leova\Desktop\Projetos\05_modelo_risco_de_credito\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FE54D6-09F1-44F0-A6C6-A16D161DC3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD6342F-DBD2-4784-B6B8-228A025A3F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="16200" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -1796,7 +1796,7 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2137,14 +2137,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2170,7 +2170,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>211</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="37.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>92</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="56.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="37.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>20</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="56.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="37.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>152</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="56.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>328</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="37.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>36</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>35</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>11</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>1</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="37.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>22</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>94</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>23</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="37.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>24</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16.149999999999999" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>30</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>25</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>210</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>26</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="37.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>27</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="37.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>28</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>31</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>33</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>34</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>32</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="37.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>232</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>203</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="37.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>274</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>114</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>99</v>
       </c>
@@ -2820,13 +2820,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D47" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="PRODUTO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D47" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B69">
     <sortCondition ref="A2:A69"/>
   </sortState>

</xml_diff>